<commit_message>
add the code of pbf feature
</commit_message>
<xml_diff>
--- a/dataset/AAindex.xlsx
+++ b/dataset/AAindex.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CE6437-BA22-45B1-8951-1D77AE303227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979F3183-E5C6-4265-A8D6-F6D7BB665009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2960" yWindow="5460" windowWidth="28800" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -177,6 +177,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -222,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -231,6 +234,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -251,9 +258,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -291,9 +298,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -326,26 +333,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -378,26 +368,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -574,14 +547,14 @@
   <dimension ref="A1:X13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.453125" customWidth="1"/>
-    <col min="23" max="23" width="21.7265625" customWidth="1"/>
-    <col min="24" max="24" width="28.26953125" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="23" max="23" width="21.77734375" customWidth="1"/>
+    <col min="24" max="24" width="28.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -793,8 +766,8 @@
       <c r="T3">
         <v>204.24</v>
       </c>
-      <c r="U3">
-        <v>0</v>
+      <c r="U3" s="4">
+        <v>130.38190476190476</v>
       </c>
       <c r="V3">
         <v>181.19</v>
@@ -867,8 +840,8 @@
       <c r="T4">
         <v>5.89</v>
       </c>
-      <c r="U4">
-        <v>0</v>
+      <c r="U4" s="4">
+        <v>5.7395238095238099</v>
       </c>
       <c r="V4">
         <v>5.66</v>
@@ -941,8 +914,8 @@
       <c r="T5">
         <v>9.44</v>
       </c>
-      <c r="U5">
-        <v>0</v>
+      <c r="U5" s="4">
+        <v>8.9119047619047631</v>
       </c>
       <c r="V5">
         <v>9.11</v>
@@ -1015,8 +988,8 @@
       <c r="T6" s="3">
         <v>2.4300000000000002</v>
       </c>
-      <c r="U6" s="3">
-        <v>0</v>
+      <c r="U6" s="5">
+        <v>2.0438095238095237</v>
       </c>
       <c r="V6" s="3">
         <v>2.2000000000000002</v>
@@ -1104,7 +1077,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1117,7 +1090,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>